<commit_message>
dsa binary search and backtracking
</commit_message>
<xml_diff>
--- a/java/TopInterview150.xlsx
+++ b/java/TopInterview150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1023EC39-AD2E-45CC-8D0F-DE3AD4876CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A873D5F-CE83-4DA5-A074-DAFEED1BD566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t>Question</t>
   </si>
@@ -189,6 +189,30 @@
   </si>
   <si>
     <t>BFS, the crux is to find the coordinates after each move. Create a helper function. All grid values are -1 unless a snake or ladder.</t>
+  </si>
+  <si>
+    <t>162. Find Peak Element</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Binary search but with custom check conditions. We partition based on the neighbors of the pivot value. An enum approach is the cleanest.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/find-peak-element/solutions/1290642/intuition-behind-conditions-complete-explanation-diagram-binary-search/?envType=study-plan-v2&amp;envId=top-interview-150 </t>
+  </si>
+  <si>
+    <t>77. Combinations</t>
+  </si>
+  <si>
+    <t>Backtracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/combinations/solutions/3845903/ex-amazon-explains-a-solution-with-a-video-python-javascript-java-and-c/?envType=study-plan-v2&amp;envId=top-interview-150 </t>
+  </si>
+  <si>
+    <t>Backtracking. Use combination.size() == k for the validity condition, then perform backtracking loop.</t>
   </si>
 </sst>
 </file>
@@ -540,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,6 +797,40 @@
       </c>
       <c r="E13" s="2" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -789,6 +847,8 @@
     <hyperlink ref="E11" r:id="rId10" xr:uid="{15073174-E93D-497D-AE3E-3F33BCF6A93E}"/>
     <hyperlink ref="E12" r:id="rId11" xr:uid="{05FFDF6D-453D-44C6-B843-815284570E82}"/>
     <hyperlink ref="E13" r:id="rId12" xr:uid="{DD16DB2C-ED65-46F1-A3C3-466D75826780}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{7EAA6900-7A17-4ABD-9769-16A48AB17D5F}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{81C64286-87A0-4E62-B1A0-6CE52255E96B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
prefix sum and linked lists
</commit_message>
<xml_diff>
--- a/java/TopInterview150.xlsx
+++ b/java/TopInterview150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A873D5F-CE83-4DA5-A074-DAFEED1BD566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FB786C-BEC2-4BC5-833F-E00C5029D600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
   <si>
     <t>Question</t>
   </si>
@@ -213,6 +213,30 @@
   </si>
   <si>
     <t>Backtracking. Use combination.size() == k for the validity condition, then perform backtracking loop.</t>
+  </si>
+  <si>
+    <t>1732. Find the Highest Altitude</t>
+  </si>
+  <si>
+    <t>Prefix Sum</t>
+  </si>
+  <si>
+    <t>Maintain a global max and local max and update in a for loop.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/find-the-highest-altitude/solutions/3759475/java-solution-beats-100/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/sort-list/solutions/46714/java-merge-sort-solution/?envType=study-plan-v2&amp;envId=top-interview-150 </t>
+  </si>
+  <si>
+    <t>148. Sort List</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>Perform merge sort on a linked list.</t>
   </si>
 </sst>
 </file>
@@ -564,15 +588,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="165.42578125" bestFit="1" customWidth="1"/>
@@ -831,6 +855,40 @@
       </c>
       <c r="E15" s="2" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -849,6 +907,8 @@
     <hyperlink ref="E13" r:id="rId12" xr:uid="{DD16DB2C-ED65-46F1-A3C3-466D75826780}"/>
     <hyperlink ref="E14" r:id="rId13" xr:uid="{7EAA6900-7A17-4ABD-9769-16A48AB17D5F}"/>
     <hyperlink ref="E15" r:id="rId14" xr:uid="{81C64286-87A0-4E62-B1A0-6CE52255E96B}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{15729C77-D197-4C00-80D4-DD4B232C6EDC}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{798F289D-ECAD-4214-97FA-B1A0031A978D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>